<commit_message>
Mainly complete data_formats vignette
</commit_message>
<xml_diff>
--- a/inst/extdata/ExcelSamples.xlsx
+++ b/inst/extdata/ExcelSamples.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24390" windowHeight="10605" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24390" windowHeight="10605" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="4col_1group" sheetId="1" r:id="rId1"/>
@@ -5709,7 +5709,7 @@
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection sqref="A1:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5991,7 +5991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
@@ -6109,7 +6109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>